<commit_message>
create migration for setup
</commit_message>
<xml_diff>
--- a/public/demo_files/Demo_DriverFormat.xlsx
+++ b/public/demo_files/Demo_DriverFormat.xlsx
@@ -16,14 +16,6 @@
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" codePage="1252"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
-  <si>
-    <t>license_no</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -95,10 +87,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -112,37 +104,35 @@
     <row r="1" spans="1:7">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>address</t>
+          <t>Address</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>joined_dt</t>
+          <t>Salary</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>salary</t>
+          <t>License No</t>
         </is>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>License Eexp</t>
+        </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>license_exp</t>
+          <t>Phone</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>phone</t>
-        </is>
-      </c>
+      <c r="G1" s="0"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>